<commit_message>
populate template of worksheet XLS
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Costing Worksheet Template.xlsx
+++ b/export/IHR Costing Tool - Costing Worksheet Template.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t>Line item ID</t>
   </si>
@@ -421,6 +421,9 @@
 The legend below defines the contents of each column and the example walks through how they apply to calculating a specific line item cost.
 In example 1 below, the cost “Conference per diems” includes the daily domestic per diem per person, times 1 annual conference lasting 3 days, times 30 people (105 USD * 1 * 3 * 30). Because this is a recurring line item, the total (9,450 USD) appears in column W, “Annual recurring costs”.
 Note that costs to increase from score 4 to 5 are highly country-specific and are not included in the IHR Costing Tool.</t>
+  </si>
+  <si>
+    <t>Target Score(s) applicable</t>
   </si>
 </sst>
 </file>
@@ -966,9 +969,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0BAA1C-8812-4BC1-86BB-AD3EF649F296}">
   <dimension ref="A1:V1500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="U2" sqref="U2:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Finalize templates for XLS export
</commit_message>
<xml_diff>
--- a/export/IHR Costing Tool - Costing Worksheet Template.xlsx
+++ b/export/IHR Costing Tool - Costing Worksheet Template.xlsx
@@ -295,9 +295,6 @@
     <t>Target score(s) applicable</t>
   </si>
   <si>
-    <t>2, 3, 4, and/or 5</t>
-  </si>
-  <si>
     <t>User's starting score for the indicator (blank by default)</t>
   </si>
   <si>
@@ -404,10 +401,6 @@
 If the default values of staff multipliers were customized in the IHR Costing Tool, the custom values are used.</t>
   </si>
   <si>
-    <t xml:space="preserve">For inputs (gray rows): The target score(s) that this input is needed to reach
-For line items (white rows): The target score(s) that this line item is needed to reach </t>
-  </si>
-  <si>
     <t>The value of the country multiplier (see column O). Adjusting this value for a line item will update the total amount calculated in the final two columns. If it is blank, it is assumed to be equal to 1.
 If country multiplier values were specified in the IHR Costing Tool, these are used. Otherwise, they can be entered manually.</t>
   </si>
@@ -423,6 +416,14 @@
   </si>
   <si>
     <t>The value of the staff multiplier (see column U). Adjusting this value for a line item will update the total amount calculated in the final two columns. If it is blank, it is assumed to be equal to 1.</t>
+  </si>
+  <si>
+    <t>For inputs (gray rows): The target score(s) that this input is needed to reach
+For line items (white rows): The target score(s) that this line item is needed to reach 
+Note that costs to increase from score 4 to 5 are highly country-specific and are not included in the IHR Costing Tool</t>
+  </si>
+  <si>
+    <t>2, 3, and/or 4</t>
   </si>
 </sst>
 </file>
@@ -37139,7 +37140,7 @@
         <v>18</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W3" s="3" t="s">
         <v>51</v>
@@ -37150,13 +37151,13 @@
         <v>20</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>39</v>
@@ -37180,40 +37181,40 @@
         <v>45</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>46</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O4" s="15" t="s">
         <v>47</v>
       </c>
       <c r="P4" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q4" s="15" t="s">
         <v>48</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S4" s="15" t="s">
         <v>49</v>
       </c>
       <c r="T4" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="U4" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V4" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W4" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:23" s="14" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -37221,13 +37222,13 @@
         <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>54</v>

</xml_diff>